<commit_message>
Feat: Add Official Data History and Dynamic Selector
</commit_message>
<xml_diff>
--- a/analisis_auditado_3540_v2.xlsx
+++ b/analisis_auditado_3540_v2.xlsx
@@ -462,56 +462,44 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>23</v>
-      </c>
       <c r="C2">
-        <v>33.8</v>
+        <v>47.5</v>
       </c>
       <c r="D2">
-        <v>10.8</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>31.7</v>
-      </c>
       <c r="C3">
-        <v>27.5</v>
+        <v>41</v>
       </c>
       <c r="D3">
-        <v>-4.2</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>17.7</v>
-      </c>
       <c r="C4">
-        <v>18.7</v>
+        <v>4.6</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>7.2</v>
-      </c>
       <c r="C5">
-        <v>6.4</v>
+        <v>4.7</v>
       </c>
       <c r="D5">
-        <v>-0.8</v>
+        <v>4.7</v>
       </c>
     </row>
   </sheetData>
@@ -558,19 +546,19 @@
         <v>33.1</v>
       </c>
       <c r="C2">
-        <v>16.8733970154216</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>1.378</v>
+        <v>3.972</v>
       </c>
       <c r="E2">
-        <v>15.9</v>
+        <v>34</v>
       </c>
       <c r="F2">
         <v>0.92</v>
       </c>
       <c r="G2">
-        <v>33.8</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -581,19 +569,19 @@
         <v>31.7</v>
       </c>
       <c r="C3">
-        <v>29.54862461022392</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>0.753</v>
+        <v>3.804</v>
       </c>
       <c r="E3">
-        <v>23.2</v>
+        <v>30</v>
       </c>
       <c r="F3">
         <v>0.93</v>
       </c>
       <c r="G3">
-        <v>27.5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -604,19 +592,19 @@
         <v>12.4</v>
       </c>
       <c r="C4">
-        <v>8.749350888203759</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>0.995</v>
+        <v>1.488</v>
       </c>
       <c r="E4">
-        <v>13.8</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>0.82</v>
       </c>
       <c r="G4">
-        <v>18.7</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -627,19 +615,19 @@
         <v>12.3</v>
       </c>
       <c r="C5">
-        <v>9.156286672362707</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>0.9429999999999999</v>
+        <v>1.476</v>
       </c>
       <c r="E5">
-        <v>4.8</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>0.85</v>
       </c>
       <c r="G5">
-        <v>6.4</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -650,19 +638,19 @@
         <v>1.9</v>
       </c>
       <c r="C6">
-        <v>1.430006354249023</v>
+        <v>10</v>
       </c>
       <c r="D6">
-        <v>0.9330000000000001</v>
+        <v>0.228</v>
       </c>
       <c r="E6">
-        <v>1.3</v>
+        <v>1.8</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>2.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -673,19 +661,19 @@
         <v>1.6</v>
       </c>
       <c r="C7">
-        <v>1.148562697273296</v>
+        <v>10</v>
       </c>
       <c r="D7">
-        <v>0.978</v>
+        <v>0.192</v>
       </c>
       <c r="E7">
-        <v>0.7</v>
+        <v>1.2</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>1.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -696,19 +684,19 @@
         <v>1.4</v>
       </c>
       <c r="C8">
-        <v>0.9734683636214173</v>
+        <v>10</v>
       </c>
       <c r="D8">
-        <v>1.01</v>
+        <v>0.168</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8">
-        <v>1.8</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -719,19 +707,19 @@
         <v>1.1</v>
       </c>
       <c r="C9">
-        <v>0.6076114328592859</v>
+        <v>10</v>
       </c>
       <c r="D9">
-        <v>1.272</v>
+        <v>0.132</v>
       </c>
       <c r="E9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9">
-        <v>1.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -742,19 +730,19 @@
         <v>0.6</v>
       </c>
       <c r="C10">
-        <v>0.6938787017390595</v>
+        <v>10</v>
       </c>
       <c r="D10">
-        <v>0.607</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="E10">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
-        <v>0.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -765,10 +753,10 @@
         <v>0.5</v>
       </c>
       <c r="C11">
-        <v>0.4255972368688463</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>0.825</v>
+        <v>0.06</v>
       </c>
       <c r="E11">
         <v>0.2</v>
@@ -777,7 +765,7 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -788,19 +776,19 @@
         <v>0.2</v>
       </c>
       <c r="C12">
-        <v>0.02736008072367857</v>
+        <v>10</v>
       </c>
       <c r="D12">
-        <v>5.134</v>
+        <v>0.024</v>
       </c>
       <c r="E12">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -811,10 +799,10 @@
         <v>0.7</v>
       </c>
       <c r="C13">
-        <v>0.6012190837835031</v>
+        <v>10</v>
       </c>
       <c r="D13">
-        <v>0.8179999999999999</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="E13">
         <v>0</v>

</xml_diff>

<commit_message>
feat: Add Technical Guide, PDF Logic, and Study Data for Cloud
</commit_message>
<xml_diff>
--- a/analisis_auditado_3540_v2.xlsx
+++ b/analisis_auditado_3540_v2.xlsx
@@ -23,7 +23,7 @@
     <t>CIS (Oficial)</t>
   </si>
   <si>
-    <t>Benedicto-Gemini</t>
+    <t>Aldabón-Gemini</t>
   </si>
   <si>
     <t>Diferencia</t>
@@ -462,44 +462,56 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2">
+        <v>23</v>
+      </c>
       <c r="C2">
-        <v>47.5</v>
+        <v>33.8</v>
       </c>
       <c r="D2">
-        <v>47.5</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3">
+        <v>31.7</v>
+      </c>
       <c r="C3">
-        <v>41</v>
+        <v>27.5</v>
       </c>
       <c r="D3">
-        <v>41</v>
+        <v>-4.2</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4">
+        <v>17.7</v>
+      </c>
       <c r="C4">
-        <v>4.6</v>
+        <v>18.7</v>
       </c>
       <c r="D4">
-        <v>4.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
+      <c r="B5">
+        <v>7.2</v>
+      </c>
       <c r="C5">
-        <v>4.7</v>
+        <v>6.4</v>
       </c>
       <c r="D5">
-        <v>4.7</v>
+        <v>-0.8</v>
       </c>
     </row>
   </sheetData>
@@ -546,19 +558,19 @@
         <v>33.1</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>675.9490378237615</v>
       </c>
       <c r="D2">
-        <v>3.972</v>
+        <v>1.378</v>
       </c>
       <c r="E2">
-        <v>34</v>
+        <v>15.9</v>
       </c>
       <c r="F2">
         <v>0.92</v>
       </c>
       <c r="G2">
-        <v>47.5</v>
+        <v>33.8</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -569,19 +581,19 @@
         <v>31.7</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>1183.719221212038</v>
       </c>
       <c r="D3">
-        <v>3.804</v>
+        <v>0.753</v>
       </c>
       <c r="E3">
-        <v>30</v>
+        <v>23.2</v>
       </c>
       <c r="F3">
         <v>0.93</v>
       </c>
       <c r="G3">
-        <v>41</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -592,19 +604,19 @@
         <v>12.4</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>350.4993872341499</v>
       </c>
       <c r="D4">
-        <v>1.488</v>
+        <v>0.995</v>
       </c>
       <c r="E4">
-        <v>10</v>
+        <v>13.8</v>
       </c>
       <c r="F4">
         <v>0.82</v>
       </c>
       <c r="G4">
-        <v>4.6</v>
+        <v>18.7</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -615,19 +627,19 @@
         <v>12.3</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>366.8012529169699</v>
       </c>
       <c r="D5">
-        <v>1.476</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>4.8</v>
       </c>
       <c r="F5">
         <v>0.85</v>
       </c>
       <c r="G5">
-        <v>4.7</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -638,19 +650,19 @@
         <v>1.9</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>57.28611840005001</v>
       </c>
       <c r="D6">
-        <v>0.228</v>
+        <v>0.9330000000000001</v>
       </c>
       <c r="E6">
-        <v>1.8</v>
+        <v>1.3</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.2</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -661,19 +673,19 @@
         <v>1.6</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>46.01147293533</v>
       </c>
       <c r="D7">
-        <v>0.192</v>
+        <v>0.978</v>
       </c>
       <c r="E7">
+        <v>0.7</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
         <v>1.2</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -684,19 +696,19 @@
         <v>1.4</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>38.99718611139</v>
       </c>
       <c r="D8">
-        <v>0.168</v>
+        <v>1.01</v>
       </c>
       <c r="E8">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8">
-        <v>0.1</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -707,19 +719,19 @@
         <v>1.1</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>24.34094112978999</v>
       </c>
       <c r="D9">
-        <v>0.132</v>
+        <v>1.272</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9">
-        <v>0.1</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -730,19 +742,19 @@
         <v>0.6</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>27.79681177289</v>
       </c>
       <c r="D10">
-        <v>0.07199999999999999</v>
+        <v>0.607</v>
       </c>
       <c r="E10">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -753,10 +765,10 @@
         <v>0.5</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>17.0494443116</v>
       </c>
       <c r="D11">
-        <v>0.06</v>
+        <v>0.825</v>
       </c>
       <c r="E11">
         <v>0.2</v>
@@ -765,7 +777,7 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -776,19 +788,19 @@
         <v>0.2</v>
       </c>
       <c r="C12">
-        <v>10</v>
+        <v>1.0960460554</v>
       </c>
       <c r="D12">
-        <v>0.024</v>
+        <v>5.134</v>
       </c>
       <c r="E12">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -799,10 +811,10 @@
         <v>0.7</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>24.0848633404</v>
       </c>
       <c r="D13">
-        <v>0.08400000000000001</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="E13">
         <v>0</v>

</xml_diff>

<commit_message>
feat: Soporte para estudios autonómicos (3543 Aragón) - Añadido estudio 3543 (Preelectoral Aragón Febrero 2026) - Soporte para partidos regionales (CHA, PAR, TERUEL EXISTE) - Extracción de todos los partidos, no solo nacionales - Documentación actualizada con diferencias Nacional/Autonómico
</commit_message>
<xml_diff>
--- a/analisis_auditado_3540_v2.xlsx
+++ b/analisis_auditado_3540_v2.xlsx
@@ -463,13 +463,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>23</v>
+        <v>35.3</v>
       </c>
       <c r="C2">
-        <v>33.8</v>
+        <v>39.1</v>
       </c>
       <c r="D2">
-        <v>10.8</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -477,13 +477,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>31.7</v>
+        <v>26.7</v>
       </c>
       <c r="C3">
         <v>27.5</v>
       </c>
       <c r="D3">
-        <v>-4.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -491,13 +491,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>17.7</v>
+        <v>15.1</v>
       </c>
       <c r="C4">
-        <v>18.7</v>
+        <v>12.9</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>-2.2</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -505,13 +505,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>7.2</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>6.4</v>
+        <v>2.3</v>
       </c>
       <c r="D5">
-        <v>-0.8</v>
+        <v>-2.7</v>
       </c>
     </row>
   </sheetData>
@@ -558,19 +558,19 @@
         <v>33.1</v>
       </c>
       <c r="C2">
-        <v>675.9490378237615</v>
+        <v>845.200004372708</v>
       </c>
       <c r="D2">
-        <v>1.378</v>
+        <v>0.987</v>
       </c>
       <c r="E2">
-        <v>15.9</v>
+        <v>27.8</v>
       </c>
       <c r="F2">
         <v>0.92</v>
       </c>
       <c r="G2">
-        <v>33.8</v>
+        <v>39.1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -581,13 +581,13 @@
         <v>31.7</v>
       </c>
       <c r="C3">
-        <v>1183.719221212038</v>
+        <v>908.1569883998282</v>
       </c>
       <c r="D3">
-        <v>0.753</v>
+        <v>0.88</v>
       </c>
       <c r="E3">
-        <v>23.2</v>
+        <v>21.5</v>
       </c>
       <c r="F3">
         <v>0.93</v>
@@ -604,19 +604,19 @@
         <v>12.4</v>
       </c>
       <c r="C4">
-        <v>350.4993872341499</v>
+        <v>366.9427356363201</v>
       </c>
       <c r="D4">
-        <v>0.995</v>
+        <v>0.852</v>
       </c>
       <c r="E4">
-        <v>13.8</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>0.82</v>
       </c>
       <c r="G4">
-        <v>18.7</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -627,19 +627,19 @@
         <v>12.3</v>
       </c>
       <c r="C5">
-        <v>366.8012529169699</v>
+        <v>397.34065786201</v>
       </c>
       <c r="D5">
-        <v>0.9429999999999999</v>
+        <v>0.78</v>
       </c>
       <c r="E5">
-        <v>4.8</v>
+        <v>2.3</v>
       </c>
       <c r="F5">
         <v>0.85</v>
       </c>
       <c r="G5">
-        <v>6.4</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -650,19 +650,19 @@
         <v>1.9</v>
       </c>
       <c r="C6">
-        <v>57.28611840005001</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0.9330000000000001</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>2.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -673,19 +673,19 @@
         <v>1.6</v>
       </c>
       <c r="C7">
-        <v>46.01147293533</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0.978</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -696,19 +696,19 @@
         <v>1.4</v>
       </c>
       <c r="C8">
-        <v>38.99718611139</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>1.01</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8">
-        <v>1.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -719,19 +719,19 @@
         <v>1.1</v>
       </c>
       <c r="C9">
-        <v>24.34094112978999</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1.272</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9">
-        <v>1.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -742,19 +742,19 @@
         <v>0.6</v>
       </c>
       <c r="C10">
-        <v>27.79681177289</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0.607</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
-        <v>0.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -765,19 +765,19 @@
         <v>0.5</v>
       </c>
       <c r="C11">
-        <v>17.0494443116</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0.825</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -788,19 +788,19 @@
         <v>0.2</v>
       </c>
       <c r="C12">
-        <v>1.0960460554</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>5.134</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -811,10 +811,10 @@
         <v>0.7</v>
       </c>
       <c r="C13">
-        <v>24.0848633404</v>
+        <v>2.73624001264</v>
       </c>
       <c r="D13">
-        <v>0.8179999999999999</v>
+        <v>6.448</v>
       </c>
       <c r="E13">
         <v>0</v>

</xml_diff>